<commit_message>
updated scripts, data file, added SQL query
</commit_message>
<xml_diff>
--- a/src/data/housing_market_Q1/processed/mw2301-january-city-toronto.xlsx
+++ b/src/data/housing_market_Q1/processed/mw2301-january-city-toronto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jobs\projects\City of Toronto\src\data\housing_market_Q1\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D6F6AA-9F47-4C21-AC09-D565467045F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F613716-B9C2-41FC-98BF-27947393A371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="6" activeTab="1" xr2:uid="{48823E95-69A9-4C80-A511-FE47259BA26E}"/>
   </bookViews>
@@ -4398,7 +4398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -4409,13 +4409,16 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="116">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -4484,7 +4487,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -5120,41 +5123,41 @@
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{2A1FB53A-A0E2-4230-94F9-203B59C5E5A2}" name="Table_Page013" displayName="Table_Page013" ref="A1:AI39" tableType="queryTable" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="35">
-    <tableColumn id="1" xr3:uid="{F440DDC7-EA66-4C03-A510-B3316185B7F4}" uniqueName="1" name="Column1" queryTableFieldId="1" headerRowDxfId="24" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{FD9AB0F1-963F-4272-B15F-5BF233DD2F98}" uniqueName="4" name="Toronto Regional Real Estate Board" queryTableFieldId="4" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{36958580-8E62-4157-AADE-3DD303874EB9}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{FDE2657E-7775-4806-A980-A415E548D111}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{F440DDC7-EA66-4C03-A510-B3316185B7F4}" uniqueName="1" name="Column1" queryTableFieldId="1" headerRowDxfId="24" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{FD9AB0F1-963F-4272-B15F-5BF233DD2F98}" uniqueName="4" name="Toronto Regional Real Estate Board" queryTableFieldId="4" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{36958580-8E62-4157-AADE-3DD303874EB9}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{FDE2657E-7775-4806-A980-A415E548D111}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="20"/>
     <tableColumn id="7" xr3:uid="{013FE8EA-2E13-4F67-8B45-301A21F9230A}" uniqueName="7" name="Column7" queryTableFieldId="7"/>
-    <tableColumn id="8" xr3:uid="{A44F23FB-1B57-4BAD-8A90-793AEAE99227}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{A44F23FB-1B57-4BAD-8A90-793AEAE99227}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="19"/>
     <tableColumn id="9" xr3:uid="{391F306A-2376-4082-8532-F678D0421560}" uniqueName="9" name="Column9" queryTableFieldId="9"/>
-    <tableColumn id="10" xr3:uid="{56A8D9D3-5423-4B37-8DE1-61F9D7476A97}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="19"/>
-    <tableColumn id="11" xr3:uid="{341E95A2-B316-4E7F-B112-60AA4764A92D}" uniqueName="11" name="Column11" queryTableFieldId="11" dataDxfId="18"/>
-    <tableColumn id="12" xr3:uid="{7713C1A4-045C-4860-AA84-B62EB45F7079}" uniqueName="12" name="Column12" queryTableFieldId="12" dataDxfId="17"/>
-    <tableColumn id="13" xr3:uid="{ABB0A4C4-3852-40BA-B7CE-23AE9814C1F4}" uniqueName="13" name="Column13" queryTableFieldId="13" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{56A8D9D3-5423-4B37-8DE1-61F9D7476A97}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{341E95A2-B316-4E7F-B112-60AA4764A92D}" uniqueName="11" name="Column11" queryTableFieldId="11" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{7713C1A4-045C-4860-AA84-B62EB45F7079}" uniqueName="12" name="Column12" queryTableFieldId="12" dataDxfId="16"/>
+    <tableColumn id="13" xr3:uid="{ABB0A4C4-3852-40BA-B7CE-23AE9814C1F4}" uniqueName="13" name="Column13" queryTableFieldId="13" dataDxfId="15"/>
     <tableColumn id="14" xr3:uid="{9E300E6A-B933-42E0-AA36-E3CE70E0B2C7}" uniqueName="14" name="Column14" queryTableFieldId="14"/>
     <tableColumn id="15" xr3:uid="{546B4149-044A-4A30-AC21-EB4D5C9291C9}" uniqueName="15" name="Column15" queryTableFieldId="15"/>
     <tableColumn id="16" xr3:uid="{15769965-D076-49AF-94A8-B11F94FF14AF}" uniqueName="16" name="Column16" queryTableFieldId="16"/>
-    <tableColumn id="17" xr3:uid="{A1B60577-C90B-4178-8AEB-98E2FF1D3DBC}" uniqueName="17" name="Column17" queryTableFieldId="17" dataDxfId="15"/>
-    <tableColumn id="18" xr3:uid="{A01021F7-E951-4FA8-8629-00A7465EDAA3}" uniqueName="18" name="Column18" queryTableFieldId="18" dataDxfId="14"/>
-    <tableColumn id="19" xr3:uid="{33C8A4DF-1DD2-4CF2-BD2E-F9EDE1A08DB7}" uniqueName="19" name="Column19" queryTableFieldId="19" dataDxfId="13"/>
+    <tableColumn id="17" xr3:uid="{A1B60577-C90B-4178-8AEB-98E2FF1D3DBC}" uniqueName="17" name="Column17" queryTableFieldId="17" dataDxfId="14"/>
+    <tableColumn id="18" xr3:uid="{A01021F7-E951-4FA8-8629-00A7465EDAA3}" uniqueName="18" name="Column18" queryTableFieldId="18" dataDxfId="13"/>
+    <tableColumn id="19" xr3:uid="{33C8A4DF-1DD2-4CF2-BD2E-F9EDE1A08DB7}" uniqueName="19" name="Column19" queryTableFieldId="19" dataDxfId="12"/>
     <tableColumn id="20" xr3:uid="{8859C2F8-491C-4F56-9967-2BF47856ECF6}" uniqueName="20" name="Column20" queryTableFieldId="20"/>
     <tableColumn id="21" xr3:uid="{E96EE1C9-E9D1-4845-99B1-6716A87D1EEC}" uniqueName="21" name="Column21" queryTableFieldId="21"/>
-    <tableColumn id="22" xr3:uid="{E9FFB942-8372-4991-8D6C-761CAF5F61CC}" uniqueName="22" name="Column22" queryTableFieldId="22" dataDxfId="12"/>
-    <tableColumn id="23" xr3:uid="{D65C2AB4-C646-485E-907B-879C8E6E0274}" uniqueName="23" name="Column23" queryTableFieldId="23" dataDxfId="11"/>
-    <tableColumn id="24" xr3:uid="{42B5E020-EFFB-401C-A0D9-79F5F25FD208}" uniqueName="24" name="Column24" queryTableFieldId="24" dataDxfId="10"/>
-    <tableColumn id="25" xr3:uid="{B44E71B1-E118-4A1F-988F-862432497395}" uniqueName="25" name="Column25" queryTableFieldId="25" dataDxfId="9"/>
+    <tableColumn id="22" xr3:uid="{E9FFB942-8372-4991-8D6C-761CAF5F61CC}" uniqueName="22" name="Column22" queryTableFieldId="22" dataDxfId="11"/>
+    <tableColumn id="23" xr3:uid="{D65C2AB4-C646-485E-907B-879C8E6E0274}" uniqueName="23" name="Column23" queryTableFieldId="23" dataDxfId="10"/>
+    <tableColumn id="24" xr3:uid="{42B5E020-EFFB-401C-A0D9-79F5F25FD208}" uniqueName="24" name="Column24" queryTableFieldId="24" dataDxfId="9"/>
+    <tableColumn id="25" xr3:uid="{B44E71B1-E118-4A1F-988F-862432497395}" uniqueName="25" name="Column25" queryTableFieldId="25" dataDxfId="8"/>
     <tableColumn id="26" xr3:uid="{1C968C56-9DB7-4084-84EA-E67357A0763D}" uniqueName="26" name="Column26" queryTableFieldId="26"/>
-    <tableColumn id="27" xr3:uid="{2173DED5-76CB-49B0-A2A3-4487393A1595}" uniqueName="27" name="Column27" queryTableFieldId="27" dataDxfId="8"/>
-    <tableColumn id="28" xr3:uid="{1FFC4DE1-612A-4BDC-837A-674313A7CF3B}" uniqueName="28" name="Column28" queryTableFieldId="28" dataDxfId="7"/>
-    <tableColumn id="29" xr3:uid="{07AF2613-5C7C-483B-8C62-C59514B42A31}" uniqueName="29" name="Column29" queryTableFieldId="29" dataDxfId="6"/>
+    <tableColumn id="27" xr3:uid="{2173DED5-76CB-49B0-A2A3-4487393A1595}" uniqueName="27" name="Column27" queryTableFieldId="27" dataDxfId="7"/>
+    <tableColumn id="28" xr3:uid="{1FFC4DE1-612A-4BDC-837A-674313A7CF3B}" uniqueName="28" name="Column28" queryTableFieldId="28" dataDxfId="6"/>
+    <tableColumn id="29" xr3:uid="{07AF2613-5C7C-483B-8C62-C59514B42A31}" uniqueName="29" name="Column29" queryTableFieldId="29" dataDxfId="5"/>
     <tableColumn id="30" xr3:uid="{DD5FA6CF-4341-4B68-B72F-A10C5E271126}" uniqueName="30" name="Column30" queryTableFieldId="30"/>
-    <tableColumn id="31" xr3:uid="{90286747-44A0-445D-9255-7634C5F35DC5}" uniqueName="31" name="Column31" queryTableFieldId="31" dataDxfId="5"/>
-    <tableColumn id="32" xr3:uid="{226C2DB5-BD45-42F4-A02C-FD39B134BB9C}" uniqueName="32" name="Column32" queryTableFieldId="32" dataDxfId="4"/>
-    <tableColumn id="33" xr3:uid="{91C401B6-CE1A-4D91-BFA1-844DDDE64693}" uniqueName="33" name="Column33" queryTableFieldId="33" dataDxfId="3"/>
+    <tableColumn id="31" xr3:uid="{90286747-44A0-445D-9255-7634C5F35DC5}" uniqueName="31" name="Column31" queryTableFieldId="31" dataDxfId="4"/>
+    <tableColumn id="32" xr3:uid="{226C2DB5-BD45-42F4-A02C-FD39B134BB9C}" uniqueName="32" name="Column32" queryTableFieldId="32" dataDxfId="3"/>
+    <tableColumn id="33" xr3:uid="{91C401B6-CE1A-4D91-BFA1-844DDDE64693}" uniqueName="33" name="Column33" queryTableFieldId="33" dataDxfId="2"/>
     <tableColumn id="34" xr3:uid="{ECA38CC2-D869-4A32-BB45-DEA3E4CA7BEE}" uniqueName="34" name="Column34" queryTableFieldId="34"/>
     <tableColumn id="35" xr3:uid="{C2B71722-AB86-4EA8-9EE9-73CA3E398669}" uniqueName="35" name="Column35" queryTableFieldId="35"/>
-    <tableColumn id="36" xr3:uid="{707BC8CD-5A9B-4627-9A28-33993E45A6D9}" uniqueName="36" name="Column36" queryTableFieldId="36" dataDxfId="2"/>
-    <tableColumn id="37" xr3:uid="{C105FDD0-1761-40CE-A5C7-16D0F9A83239}" uniqueName="37" name="Column37" queryTableFieldId="37" dataDxfId="1"/>
+    <tableColumn id="36" xr3:uid="{707BC8CD-5A9B-4627-9A28-33993E45A6D9}" uniqueName="36" name="Column36" queryTableFieldId="36" dataDxfId="1"/>
+    <tableColumn id="37" xr3:uid="{C105FDD0-1761-40CE-A5C7-16D0F9A83239}" uniqueName="37" name="Column37" queryTableFieldId="37" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -11025,7 +11028,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A22" sqref="A22:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11651,31 +11654,31 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="B22" t="s">
-        <v>334</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="B22" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="C22" s="6">
+        <v>0</v>
+      </c>
+      <c r="D22" s="6">
+        <v>0</v>
+      </c>
+      <c r="E22" s="6">
+        <v>0</v>
+      </c>
+      <c r="F22" s="6" t="s">
         <v>335</v>
       </c>
       <c r="G22" s="4">
         <v>3</v>
       </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
+      <c r="H22" s="6">
+        <v>0</v>
+      </c>
+      <c r="I22" s="6">
         <v>0</v>
       </c>
     </row>

</xml_diff>